<commit_message>
Email sent task marked off
</commit_message>
<xml_diff>
--- a/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
+++ b/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t xml:space="preserve">CITS3200 Project Billed Hours Record for Seb
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t xml:space="preserve">Booked room for first meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send email to client asking for meeting/information</t>
   </si>
 </sst>
 </file>
@@ -186,20 +189,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -237,14 +240,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -454,8 +449,8 @@
   </sheetPr>
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -551,7 +546,7 @@
         <f aca="false">IF(G4&lt;&gt;"ERROR",G4)</f>
         <v>0.0833333333333333</v>
       </c>
-      <c r="I4" s="14" t="n">
+      <c r="I4" s="1" t="n">
         <f aca="false">((D4+E4)-(B4+C4))*24</f>
         <v>0.0833333333333333</v>
       </c>
@@ -575,7 +570,7 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="15" t="n">
+      <c r="G5" s="13" t="n">
         <f aca="false">IF(I5&gt;0,I5,IF(I5=0, " ", "ERROR"))</f>
         <v>1.8225</v>
       </c>
@@ -621,21 +616,35 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="G7" s="13" t="str">
+      <c r="A7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>44404</v>
+      </c>
+      <c r="C7" s="12" t="n">
+        <v>0.645833333333333</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>44404</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>0.65625</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="13" t="n">
         <f aca="false">IF(I7&gt;0,I7,IF(I7=0, " ", "ERROR"))</f>
-        <v> </v>
-      </c>
-      <c r="H7" s="1" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <f aca="false">IF(AND(G7&lt;&gt;" ",G7&lt;&gt;"ERROR",H6&lt;&gt;" ", H6&lt;&gt;"ERROR"),G7+H6," ")</f>
-        <v> </v>
+        <v>2.23916666666667</v>
       </c>
       <c r="I7" s="1" t="n">
         <f aca="false">((D7+E7)-(B7+C7))*24</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,14 +1065,14 @@
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="5" t="s">
         <v>4</v>
       </c>
@@ -1080,16 +1089,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="5"/>
@@ -1665,14 +1674,14 @@
       <c r="A65" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16" t="s">
+      <c r="C65" s="14"/>
+      <c r="D65" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="16"/>
+      <c r="E65" s="14"/>
       <c r="F65" s="5" t="s">
         <v>4</v>
       </c>
@@ -1689,16 +1698,16 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C66" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="18" t="s">
+      <c r="E66" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F66" s="5"/>
@@ -2161,14 +2170,14 @@
       <c r="A99" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16" t="s">
+      <c r="C99" s="14"/>
+      <c r="D99" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E99" s="16"/>
+      <c r="E99" s="14"/>
       <c r="F99" s="5" t="s">
         <v>4</v>
       </c>
@@ -2185,16 +2194,16 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5"/>
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="C100" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D100" s="17" t="s">
+      <c r="D100" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="18" t="s">
+      <c r="E100" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F100" s="5"/>

</xml_diff>

<commit_message>
Another thing off my todo list
</commit_message>
<xml_diff>
--- a/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
+++ b/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t xml:space="preserve">CITS3200 Project Billed Hours Record for Seb
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">Send email to client asking for meeting/information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup branch rules on the github repo</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -648,21 +651,35 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="G8" s="13" t="str">
+      <c r="A8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>44404</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <v>0.660416666666667</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>44404</v>
+      </c>
+      <c r="E8" s="12" t="n">
+        <v>0.663888888888889</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="13" t="n">
         <f aca="false">IF(I8&gt;0,I8,IF(I8=0, " ", "ERROR"))</f>
-        <v> </v>
-      </c>
-      <c r="H8" s="1" t="str">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <f aca="false">IF(AND(G8&lt;&gt;" ",G8&lt;&gt;"ERROR",H7&lt;&gt;" ", H7&lt;&gt;"ERROR"),G8+H7," ")</f>
-        <v> </v>
+        <v>2.3225</v>
       </c>
       <c r="I8" s="1" t="n">
         <f aca="false">((D8+E8)-(B8+C8))*24</f>
-        <v>0</v>
+        <v>0.0833333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated Quans timesheet to reflect actual meeting time
(he had put down less than what the actual meeting time was)
</commit_message>
<xml_diff>
--- a/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
+++ b/Organisational/Members/Seb/Booked_Hours_Seb.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t xml:space="preserve">CITS3200 Project Billed Hours Record for Seb
 Each time you do some work on the project, note the week number, start and end date and hour, plus a brief description of the activity. At the end of each week send a copy of the sheet as it currently stands to your group's manager for recording on the group TimeSheet. Date in the form DD/MM/YY and time as XX:YY (24hr clock)</t>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">Send response email to cleint trying to organise meeting for monday morning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on improving the github setup – added project/task board and issues, and switched to an organsiation instead of personal as that gives us better project management features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sent email to auditor asking to organise a meeting</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,6 +533,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="5"/>
       <c r="H3" s="8"/>
+      <c r="L3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -753,39 +760,67 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="G11" s="13" t="str">
+      <c r="A11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>44405</v>
+      </c>
+      <c r="C11" s="12" t="n">
+        <v>0.756944444444444</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>44405</v>
+      </c>
+      <c r="E11" s="12" t="n">
+        <v>0.933333333333333</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="13" t="n">
         <f aca="false">IF(I11&gt;0,I11,IF(I11=0, " ", "ERROR"))</f>
-        <v> </v>
-      </c>
-      <c r="H11" s="1" t="str">
+        <v>4.23333333333333</v>
+      </c>
+      <c r="H11" s="1" t="n">
         <f aca="false">IF(AND(G11&lt;&gt;" ",G11&lt;&gt;"ERROR",H10&lt;&gt;" ", H10&lt;&gt;"ERROR"),G11+H10," ")</f>
-        <v> </v>
+        <v>7.4725</v>
       </c>
       <c r="I11" s="1" t="n">
         <f aca="false">((D11+E11)-(B11+C11))*24</f>
-        <v>0</v>
+        <v>4.23333333333333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="G12" s="13" t="str">
+      <c r="A12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>44408</v>
+      </c>
+      <c r="C12" s="12" t="n">
+        <v>0.430555555555556</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>44408</v>
+      </c>
+      <c r="E12" s="12" t="n">
+        <v>0.434027777777778</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="13" t="n">
         <f aca="false">IF(I12&gt;0,I12,IF(I12=0, " ", "ERROR"))</f>
-        <v> </v>
-      </c>
-      <c r="H12" s="1" t="str">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <f aca="false">IF(AND(G12&lt;&gt;" ",G12&lt;&gt;"ERROR",H11&lt;&gt;" ", H11&lt;&gt;"ERROR"),G12+H11," ")</f>
-        <v> </v>
+        <v>7.55583333333333</v>
       </c>
       <c r="I12" s="1" t="n">
         <f aca="false">((D12+E12)-(B12+C12))*24</f>
-        <v>0</v>
+        <v>0.0833333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,7 +2794,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="L3 D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2782,7 +2817,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>